<commit_message>
Zeitplan Update (for real for today)
</commit_message>
<xml_diff>
--- a/Forschungsseminar_Zeittabelle.xlsx
+++ b/Forschungsseminar_Zeittabelle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Master Thesis\Master-Thesis-TD-AI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8640CF7-D992-4C8C-8A41-9E98DA60B658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD02699F-8D50-4EA3-9D2A-5D8933B480F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeiterfassung" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Name, Vorname: Müller, Stefan</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>Brainstorming Anpassung Observations, Mehrere Felder zum spawnen machen für Training WIP</t>
+  </si>
+  <si>
+    <t>FileWriter erstellt mehr Einsicht in Observationen, mehr Training</t>
   </si>
 </sst>
 </file>
@@ -626,7 +629,7 @@
       </c>
       <c r="B4" s="2">
         <f>SUM(B6:B129)</f>
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -975,8 +978,12 @@
       <c r="A33" s="24">
         <v>45125</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="7"/>
+      <c r="B33" s="9">
+        <v>6</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
     </row>
@@ -2278,7 +2285,7 @@
       </c>
       <c r="B3" s="17">
         <f>SUM(Zeiterfassung!B12:B41)</f>
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2344,7 +2351,7 @@
       </c>
       <c r="B12" s="19">
         <f>SUM(B2:B8)</f>
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Zeitplan Update (heute und Gestern)
Training, TowerSelect Training hat die TowerSelect Action ohne Observationen jetzt
</commit_message>
<xml_diff>
--- a/Forschungsseminar_Zeittabelle.xlsx
+++ b/Forschungsseminar_Zeittabelle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Master Thesis\Master-Thesis-TD-AI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FB939F-98EF-4AE0-9F76-29299240B271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E87F24-EA7F-4456-8B2A-4738A47E9160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeiterfassung" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Name, Vorname: Müller, Stefan</t>
   </si>
@@ -182,6 +182,12 @@
   </si>
   <si>
     <t>Bugfix + Training mit versch. Config Variablenwerten</t>
+  </si>
+  <si>
+    <t>Bugfix + erneutes Training</t>
+  </si>
+  <si>
+    <t>Simpleres Training anders aufgebaut gutes Resultat</t>
   </si>
 </sst>
 </file>
@@ -628,7 +634,7 @@
   <dimension ref="A1:E193"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,7 +674,7 @@
       </c>
       <c r="B4" s="2">
         <f>SUM(B6:B129)</f>
-        <v>202</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1251,8 +1257,12 @@
       <c r="A53" s="24">
         <v>45145</v>
       </c>
-      <c r="B53" s="9"/>
-      <c r="C53" s="7"/>
+      <c r="B53" s="9">
+        <v>5</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
     </row>
@@ -1260,8 +1270,12 @@
       <c r="A54" s="24">
         <v>45146</v>
       </c>
-      <c r="B54" s="9"/>
-      <c r="C54" s="7"/>
+      <c r="B54" s="9">
+        <v>7</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="D54" s="7"/>
       <c r="E54" s="7"/>
     </row>
@@ -1269,8 +1283,12 @@
       <c r="A55" s="24">
         <v>45147</v>
       </c>
-      <c r="B55" s="9"/>
-      <c r="C55" s="7"/>
+      <c r="B55" s="9">
+        <v>8</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>49</v>
+      </c>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
     </row>
@@ -2383,7 +2401,7 @@
       </c>
       <c r="B4" s="17">
         <f>SUM(Zeiterfassung!B42:B53)</f>
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2392,7 +2410,7 @@
       </c>
       <c r="B5" s="17">
         <f>SUM(Zeiterfassung!B54:B56)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2440,7 +2458,7 @@
       </c>
       <c r="B12" s="19">
         <f>SUM(B2:B8)</f>
-        <v>202</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>